<commit_message>
Late commit due to confusion in db setup
</commit_message>
<xml_diff>
--- a/SampleVarList.xlsx
+++ b/SampleVarList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scerj047\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/estherspiteri/Masters/Masters-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AB81E6E-7933-4F72-9027-62B05ADD464A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00348EB9-A180-B348-9CE4-D598D26E7CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0E7ED75A-1A74-408B-8658-674D689ED589}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0E7ED75A-1A74-408B-8658-674D689ED589}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2735,27 +2735,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A22DEF7-C682-406C-AC75-C463E18B4FE4}">
   <dimension ref="A1:I461"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G319" sqref="G319"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>92</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>93</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>102</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>103</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>106</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>110</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>112</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>114</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>117</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>119</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>125</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>126</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>128</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>129</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>130</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>139</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>140</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>143</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>149</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>151</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>152</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>153</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>156</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>158</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>159</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>161</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>162</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>164</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>165</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>166</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>167</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>170</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>172</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>173</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>176</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>177</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>179</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>181</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>184</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>185</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>186</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>187</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>188</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>189</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>190</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>191</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>192</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>195</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>198</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>199</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>200</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>201</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>202</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>203</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>205</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>206</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>209</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>210</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>211</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>212</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>213</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>215</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>218</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>219</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>220</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>221</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>222</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>223</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>224</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>225</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>226</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>228</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>230</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>231</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>232</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>233</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>234</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>235</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>237</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>241</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>244</v>
       </c>
@@ -6268,7 +6268,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>247</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>248</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>249</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>251</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>253</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>255</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>257</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>259</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>260</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>262</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>263</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>264</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>266</v>
       </c>
@@ -6606,7 +6606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>267</v>
       </c>
@@ -6632,7 +6632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>268</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>272</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>274</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>275</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>276</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>277</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>278</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>280</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>282</v>
       </c>
@@ -6866,7 +6866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>284</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>285</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>286</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>288</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>290</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>292</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>296</v>
       </c>
@@ -7048,7 +7048,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>297</v>
       </c>
@@ -7074,7 +7074,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>299</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>301</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>302</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>304</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>305</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>306</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>308</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>310</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>312</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>314</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>315</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>318</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>319</v>
       </c>
@@ -7412,7 +7412,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>320</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>321</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>324</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>324</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>326</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>327</v>
       </c>
@@ -7568,7 +7568,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>329</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>331</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>332</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>334</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>335</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>337</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>338</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>339</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>340</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>341</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>342</v>
       </c>
@@ -7854,7 +7854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>344</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>345</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>346</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>347</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>349</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>350</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>351</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>352</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>353</v>
       </c>
@@ -8088,7 +8088,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>355</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>359</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>360</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>364</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>366</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>368</v>
       </c>
@@ -8296,7 +8296,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>369</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>370</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>371</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>374</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>376</v>
       </c>
@@ -8426,7 +8426,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>377</v>
       </c>
@@ -8452,7 +8452,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>379</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>380</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>381</v>
       </c>
@@ -8530,7 +8530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>383</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>384</v>
       </c>
@@ -8582,7 +8582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>385</v>
       </c>
@@ -8608,7 +8608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>386</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>387</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>388</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>389</v>
       </c>
@@ -8712,7 +8712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>391</v>
       </c>
@@ -8738,7 +8738,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>395</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>396</v>
       </c>
@@ -8790,7 +8790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>397</v>
       </c>
@@ -8816,7 +8816,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>398</v>
       </c>
@@ -8842,7 +8842,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>401</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>402</v>
       </c>
@@ -8894,7 +8894,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>403</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>405</v>
       </c>
@@ -8946,7 +8946,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>406</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>407</v>
       </c>
@@ -8998,7 +8998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>409</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>410</v>
       </c>
@@ -9050,7 +9050,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>411</v>
       </c>
@@ -9076,7 +9076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>412</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>415</v>
       </c>
@@ -9128,7 +9128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>418</v>
       </c>
@@ -9154,7 +9154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>420</v>
       </c>
@@ -9180,7 +9180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>421</v>
       </c>
@@ -9206,7 +9206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>423</v>
       </c>
@@ -9232,7 +9232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>425</v>
       </c>
@@ -9258,7 +9258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>426</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>427</v>
       </c>
@@ -9310,7 +9310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>431</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>433</v>
       </c>
@@ -9362,7 +9362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>434</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>436</v>
       </c>
@@ -9414,7 +9414,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>438</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>440</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>442</v>
       </c>
@@ -9492,7 +9492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>443</v>
       </c>
@@ -9518,7 +9518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>445</v>
       </c>
@@ -9544,7 +9544,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>446</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>447</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>448</v>
       </c>
@@ -9622,7 +9622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>450</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>452</v>
       </c>
@@ -9674,7 +9674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>453</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>454</v>
       </c>
@@ -9726,7 +9726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>455</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>456</v>
       </c>
@@ -9778,7 +9778,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>458</v>
       </c>
@@ -9804,7 +9804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>460</v>
       </c>
@@ -9830,7 +9830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>461</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>462</v>
       </c>
@@ -9882,7 +9882,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>464</v>
       </c>
@@ -9908,7 +9908,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>468</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>470</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>472</v>
       </c>
@@ -9986,7 +9986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>473</v>
       </c>
@@ -10012,7 +10012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>474</v>
       </c>
@@ -10038,7 +10038,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>477</v>
       </c>
@@ -10064,7 +10064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>478</v>
       </c>
@@ -10090,7 +10090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>480</v>
       </c>
@@ -10116,7 +10116,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>481</v>
       </c>
@@ -10142,7 +10142,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>482</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>484</v>
       </c>
@@ -10194,7 +10194,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>486</v>
       </c>
@@ -10220,7 +10220,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>488</v>
       </c>
@@ -10246,7 +10246,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>490</v>
       </c>
@@ -10272,7 +10272,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>493</v>
       </c>
@@ -10298,7 +10298,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>494</v>
       </c>
@@ -10324,7 +10324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>495</v>
       </c>
@@ -10350,7 +10350,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>497</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>498</v>
       </c>
@@ -10402,7 +10402,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>499</v>
       </c>
@@ -10428,7 +10428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>500</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>501</v>
       </c>
@@ -10480,7 +10480,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>502</v>
       </c>
@@ -10506,7 +10506,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>503</v>
       </c>
@@ -10532,7 +10532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>505</v>
       </c>
@@ -10558,7 +10558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>508</v>
       </c>
@@ -10584,7 +10584,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>510</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>514</v>
       </c>
@@ -10636,7 +10636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>515</v>
       </c>
@@ -10662,7 +10662,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>518</v>
       </c>
@@ -10688,7 +10688,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>521</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>522</v>
       </c>
@@ -10740,7 +10740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>527</v>
       </c>
@@ -10766,7 +10766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>528</v>
       </c>
@@ -10792,7 +10792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>529</v>
       </c>
@@ -10818,7 +10818,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>531</v>
       </c>
@@ -10844,7 +10844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>532</v>
       </c>
@@ -10870,7 +10870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>534</v>
       </c>
@@ -10896,7 +10896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>537</v>
       </c>
@@ -10922,7 +10922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>539</v>
       </c>
@@ -10951,7 +10951,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>541</v>
       </c>
@@ -10977,7 +10977,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>541</v>
       </c>
@@ -11006,7 +11006,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>545</v>
       </c>
@@ -11032,7 +11032,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>546</v>
       </c>
@@ -11058,7 +11058,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>547</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>549</v>
       </c>
@@ -11110,7 +11110,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>550</v>
       </c>
@@ -11139,7 +11139,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>555</v>
       </c>
@@ -11165,7 +11165,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>556</v>
       </c>
@@ -11191,7 +11191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>558</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>559</v>
       </c>
@@ -11243,7 +11243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>561</v>
       </c>
@@ -11269,7 +11269,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>562</v>
       </c>
@@ -11295,7 +11295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>563</v>
       </c>
@@ -11321,7 +11321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>565</v>
       </c>
@@ -11347,7 +11347,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>566</v>
       </c>
@@ -11373,7 +11373,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>567</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>569</v>
       </c>
@@ -11425,7 +11425,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>571</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>572</v>
       </c>
@@ -11477,7 +11477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>573</v>
       </c>
@@ -11503,7 +11503,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>574</v>
       </c>
@@ -11529,7 +11529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>575</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>576</v>
       </c>
@@ -11581,7 +11581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>577</v>
       </c>
@@ -11607,7 +11607,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>579</v>
       </c>
@@ -11633,7 +11633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>580</v>
       </c>
@@ -11659,7 +11659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>581</v>
       </c>
@@ -11685,7 +11685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>582</v>
       </c>
@@ -11711,7 +11711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>583</v>
       </c>
@@ -11737,7 +11737,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>585</v>
       </c>
@@ -11763,7 +11763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>586</v>
       </c>
@@ -11789,7 +11789,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>587</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>588</v>
       </c>
@@ -11841,7 +11841,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>590</v>
       </c>
@@ -11867,7 +11867,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>591</v>
       </c>
@@ -11893,7 +11893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>592</v>
       </c>
@@ -11919,7 +11919,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>593</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>597</v>
       </c>
@@ -11971,7 +11971,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>599</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>601</v>
       </c>
@@ -12023,7 +12023,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>602</v>
       </c>
@@ -12049,7 +12049,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>603</v>
       </c>
@@ -12075,7 +12075,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>605</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>607</v>
       </c>
@@ -12127,7 +12127,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>611</v>
       </c>
@@ -12153,7 +12153,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>613</v>
       </c>
@@ -12179,7 +12179,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>614</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>615</v>
       </c>
@@ -12231,7 +12231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>617</v>
       </c>
@@ -12257,7 +12257,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>619</v>
       </c>
@@ -12283,7 +12283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>621</v>
       </c>
@@ -12309,7 +12309,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>622</v>
       </c>
@@ -12335,7 +12335,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>624</v>
       </c>
@@ -12361,7 +12361,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>625</v>
       </c>
@@ -12387,7 +12387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>626</v>
       </c>
@@ -12416,7 +12416,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>630</v>
       </c>
@@ -12442,7 +12442,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>634</v>
       </c>
@@ -12468,7 +12468,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>636</v>
       </c>
@@ -12494,7 +12494,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>637</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>641</v>
       </c>
@@ -12546,7 +12546,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>642</v>
       </c>
@@ -12572,7 +12572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>643</v>
       </c>
@@ -12598,7 +12598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>647</v>
       </c>
@@ -12624,7 +12624,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>648</v>
       </c>
@@ -12650,7 +12650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>650</v>
       </c>
@@ -12676,7 +12676,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>651</v>
       </c>
@@ -12702,7 +12702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>653</v>
       </c>
@@ -12728,7 +12728,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>653</v>
       </c>
@@ -12754,7 +12754,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>655</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>656</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>658</v>
       </c>
@@ -12832,7 +12832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>660</v>
       </c>
@@ -12858,7 +12858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>662</v>
       </c>
@@ -12884,7 +12884,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>664</v>
       </c>
@@ -12910,7 +12910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>665</v>
       </c>
@@ -12936,7 +12936,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>667</v>
       </c>
@@ -12962,7 +12962,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>668</v>
       </c>
@@ -12988,7 +12988,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>671</v>
       </c>
@@ -13014,7 +13014,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>672</v>
       </c>
@@ -13040,7 +13040,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>673</v>
       </c>
@@ -13066,7 +13066,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>674</v>
       </c>
@@ -13092,7 +13092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>676</v>
       </c>
@@ -13118,7 +13118,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>677</v>
       </c>
@@ -13144,7 +13144,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>681</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>682</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>684</v>
       </c>
@@ -13222,7 +13222,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>686</v>
       </c>
@@ -13248,7 +13248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>688</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>689</v>
       </c>
@@ -13300,7 +13300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>690</v>
       </c>
@@ -13326,7 +13326,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>691</v>
       </c>
@@ -13352,7 +13352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>694</v>
       </c>
@@ -13378,7 +13378,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>695</v>
       </c>
@@ -13404,7 +13404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>696</v>
       </c>
@@ -13430,7 +13430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>697</v>
       </c>
@@ -13456,7 +13456,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>698</v>
       </c>
@@ -13482,7 +13482,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>699</v>
       </c>
@@ -13508,7 +13508,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>700</v>
       </c>
@@ -13534,7 +13534,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>702</v>
       </c>
@@ -13560,7 +13560,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>703</v>
       </c>
@@ -13586,7 +13586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>704</v>
       </c>
@@ -13612,7 +13612,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>705</v>
       </c>
@@ -13638,7 +13638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>707</v>
       </c>
@@ -13664,7 +13664,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>707</v>
       </c>
@@ -13690,7 +13690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>707</v>
       </c>
@@ -13716,7 +13716,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>708</v>
       </c>
@@ -13742,7 +13742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>709</v>
       </c>
@@ -13768,7 +13768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>710</v>
       </c>
@@ -13794,7 +13794,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>712</v>
       </c>
@@ -13820,7 +13820,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>713</v>
       </c>
@@ -13846,7 +13846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>713</v>
       </c>
@@ -13872,7 +13872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>718</v>
       </c>
@@ -13898,7 +13898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>718</v>
       </c>
@@ -13924,7 +13924,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>723</v>
       </c>
@@ -13950,7 +13950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>724</v>
       </c>
@@ -13976,7 +13976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>725</v>
       </c>
@@ -14002,7 +14002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>728</v>
       </c>
@@ -14028,7 +14028,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>730</v>
       </c>
@@ -14054,7 +14054,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>731</v>
       </c>
@@ -14080,7 +14080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>733</v>
       </c>
@@ -14106,7 +14106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>735</v>
       </c>
@@ -14132,7 +14132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>737</v>
       </c>
@@ -14158,7 +14158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>740</v>
       </c>
@@ -14184,7 +14184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>741</v>
       </c>
@@ -14210,7 +14210,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>743</v>
       </c>
@@ -14236,7 +14236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>745</v>
       </c>
@@ -14262,7 +14262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
         <v>746</v>
       </c>
@@ -14288,7 +14288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
         <v>750</v>
       </c>
@@ -14314,7 +14314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>752</v>
       </c>
@@ -14340,7 +14340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>754</v>
       </c>
@@ -14366,7 +14366,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>755</v>
       </c>
@@ -14392,7 +14392,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>757</v>
       </c>
@@ -14418,7 +14418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>759</v>
       </c>
@@ -14444,7 +14444,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="452" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>760</v>
       </c>
@@ -14470,7 +14470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>761</v>
       </c>
@@ -14496,7 +14496,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>764</v>
       </c>
@@ -14522,7 +14522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="455" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>766</v>
       </c>
@@ -14548,7 +14548,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>767</v>
       </c>
@@ -14574,7 +14574,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="457" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>769</v>
       </c>
@@ -14600,7 +14600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>774</v>
       </c>
@@ -14626,7 +14626,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>778</v>
       </c>
@@ -14652,7 +14652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>780</v>
       </c>
@@ -14678,7 +14678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>781</v>
       </c>

</xml_diff>